<commit_message>
Kicad 3D model changed
</commit_message>
<xml_diff>
--- a/PCB components list.xlsx
+++ b/PCB components list.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rubén\Desktop\Humanoide\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rubén\Documents\GitHub\zord-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -110,9 +110,6 @@
     <t>array 4 resistor 0603 1k</t>
   </si>
   <si>
-    <t>coil BLM21</t>
-  </si>
-  <si>
     <t>diode CD1206-S01575</t>
   </si>
   <si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>inductor BLM21</t>
   </si>
 </sst>
 </file>
@@ -329,6 +329,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -336,24 +354,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -674,7 +674,7 @@
   <dimension ref="A2:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,24 +687,24 @@
     <col min="6" max="6" width="80.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="D2" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>45</v>
+      <c r="F2" s="22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -880,7 +880,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C11" s="3">
         <v>25</v>
@@ -943,7 +943,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="3">
         <v>100</v>
@@ -985,7 +985,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="3">
         <v>5</v>
@@ -1006,7 +1006,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="3">
         <v>10</v>
@@ -1028,7 +1028,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
@@ -1050,7 +1050,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="4">
         <v>10</v>
@@ -1068,48 +1068,48 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
       <c r="G20" s="15"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="17"/>
-      <c r="C21" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
+      <c r="C21" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
-      <c r="D23" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="22">
+      <c r="D23" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="19">
         <f>SUM(E3:E19)</f>
         <v>51.041299999999993</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
-      <c r="D24" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="22">
+      <c r="D24" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="19">
         <f>5*1.21</f>
         <v>6.05</v>
       </c>
@@ -1119,10 +1119,10 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="14"/>
-      <c r="D26" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="24">
+      <c r="D26" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="21">
         <f>E23+E24</f>
         <v>57.09129999999999</v>
       </c>

</xml_diff>